<commit_message>
Update coordinates for Whiteley map
</commit_message>
<xml_diff>
--- a/amnh/mapping/maps/coordinates.xlsx
+++ b/amnh/mapping/maps/coordinates.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/BantuMigration/amnh/mapping/maps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\amnh\mapping\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3752B89D-336D-7042-91E2-DCFD5FBDC58B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972C4CFE-B11C-4DEA-A89F-C0F68FCF282A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1A7ED33D-DE51-4E76-A3DA-B1B683C9C880}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1A7ED33D-DE51-4E76-A3DA-B1B683C9C880}"/>
   </bookViews>
   <sheets>
     <sheet name="c coordinates" sheetId="1" r:id="rId1"/>
     <sheet name="d coordinates" sheetId="2" r:id="rId2"/>
+    <sheet name="whiteley coordinates" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>Point</t>
   </si>
@@ -125,6 +126,156 @@
   </si>
   <si>
     <t>9_outjet13-outjet14</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>red_start</t>
+  </si>
+  <si>
+    <t>red_midpoint</t>
+  </si>
+  <si>
+    <t>red_end</t>
+  </si>
+  <si>
+    <t>orange_branchpoint</t>
+  </si>
+  <si>
+    <t>orange_end_1</t>
+  </si>
+  <si>
+    <t>orange_end_2</t>
+  </si>
+  <si>
+    <t>yellow_start</t>
+  </si>
+  <si>
+    <t>yellow_end</t>
+  </si>
+  <si>
+    <t>green_branchpoint</t>
+  </si>
+  <si>
+    <t>green_start</t>
+  </si>
+  <si>
+    <t>green_end_1</t>
+  </si>
+  <si>
+    <t>green_end_2</t>
+  </si>
+  <si>
+    <t>pink_start</t>
+  </si>
+  <si>
+    <t>pink_branchpoint_1</t>
+  </si>
+  <si>
+    <t>pink_end_1</t>
+  </si>
+  <si>
+    <t>pink_branchpoint_2</t>
+  </si>
+  <si>
+    <t>pink_end_2</t>
+  </si>
+  <si>
+    <t>pink_end_3</t>
+  </si>
+  <si>
+    <t>blue_start</t>
+  </si>
+  <si>
+    <t>blue_branchpoint_1</t>
+  </si>
+  <si>
+    <t>blue_end_1</t>
+  </si>
+  <si>
+    <t>blue_branchpoint_2</t>
+  </si>
+  <si>
+    <t>blue_end_2</t>
+  </si>
+  <si>
+    <t>blue_end_3</t>
   </si>
 </sst>
 </file>
@@ -479,13 +630,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695B2B5E-1E83-49F4-8638-02A74A55756E}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="179" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -507,7 +658,7 @@
         <v>10.008698000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -518,7 +669,7 @@
         <v>10.462020000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -529,7 +680,7 @@
         <v>17.828506999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -540,7 +691,7 @@
         <v>20.246224999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -551,7 +702,7 @@
         <v>18.602931999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -562,7 +713,7 @@
         <v>21.927295000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -573,7 +724,7 @@
         <v>27.027179</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -584,7 +735,7 @@
         <v>27.971591</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -595,7 +746,7 @@
         <v>32.297041</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -606,7 +757,7 @@
         <v>33.147019999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -617,7 +768,7 @@
         <v>33.845891999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -628,7 +779,7 @@
         <v>31.428173000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -639,7 +790,7 @@
         <v>31.711500000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -650,7 +801,7 @@
         <v>30.427087</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -661,7 +812,7 @@
         <v>33.411458000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -672,7 +823,7 @@
         <v>39.210205000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -683,7 +834,7 @@
         <v>38.511333</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -694,7 +845,7 @@
         <v>31.560392</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -712,345 +863,661 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79C9DC9-5CE5-4844-B701-32E51CBBCB7F}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
         <v>5.3977839999999997</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>10.230079</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
         <v>2.8473229999999998</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>11.575024000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
         <v>4.0385499999999999</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>13.090456</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
         <v>-0.48544900000000002</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>13.317771</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
         <v>-2.3412069999999998</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>16.234977000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
         <v>-0.94004200000000004</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>19.322669999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
         <v>-3.4762979999999999</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>16.329692000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
         <v>-3.8732799999999998</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>15.496204000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
         <v>-4.3834090000000003</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>14.378572999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
         <v>-2.8142990000000001</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>13.564029</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
         <v>-5.9492330000000004</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>18.223981999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13">
         <v>-7.3791279999999997</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>21.198017</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
         <v>-12.175259</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>21.728418000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
         <v>-14.038558</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>20.857043999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
         <v>-6.4953390000000004</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>25.498054</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17">
         <v>-5.3460049999999999</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>30.006464000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
         <v>-5.836176</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>31.881810999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19">
         <v>-3.249374</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>31.446124000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20">
         <v>-1.9626170000000001</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>33.169927999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21">
         <v>-7.6420529999999998</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>35.708275999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22">
         <v>-5.6665479999999997</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>37.716222999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23">
         <v>-4.3267449999999998</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>37.905652000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
         <v>-3.2871990000000002</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>37.829881</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25">
         <v>-0.88322000000000001</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>37.829881</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
         <v>-9.0663979999999995</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>36.257620000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27">
         <v>-9.9258220000000001</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>36.750135999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28">
         <v>-10.969023</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>38.417110999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
         <v>-11.396437000000001</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>34.685360000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30">
         <v>-18.958936999999999</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>29.172975999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99520C0-D302-4280-9EA3-93C31CA68404}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>